<commit_message>
Update CDP and CDM-4
Atualização do CDP conforme observações do CDM-4 e atualização do CDM-4
com o preenchimento da Sessão 2, anteriormente esquecida.
</commit_message>
<xml_diff>
--- a/Projeto/GPR/PG2016-1-CDM-4.xlsx
+++ b/Projeto/GPR/PG2016-1-CDM-4.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>1. Acompanhamento de Execução</t>
   </si>
@@ -133,6 +133,15 @@
       </rPr>
       <t>A atividade "AT23" ainda não foi concluída, será planejado novo prazo para término dessa atividade e posteriomente os valores de esforço e custo serão atualizados.</t>
     </r>
+  </si>
+  <si>
+    <t>Não Comprimento do Cronograma</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Sim</t>
   </si>
 </sst>
 </file>
@@ -728,7 +737,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:I14"/>
+      <selection activeCell="A18" sqref="A18:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1020,12 +1029,18 @@
       <c r="I16" s="26"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="15"/>
+      <c r="A17" s="15" t="s">
+        <v>34</v>
+      </c>
       <c r="B17" s="17"/>
       <c r="C17" s="16"/>
-      <c r="D17" s="15"/>
+      <c r="D17" s="15" t="s">
+        <v>35</v>
+      </c>
       <c r="E17" s="16"/>
-      <c r="F17" s="15"/>
+      <c r="F17" s="15" t="s">
+        <v>36</v>
+      </c>
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
       <c r="I17" s="16"/>

</xml_diff>